<commit_message>
implementado a animação de andar do player
</commit_message>
<xml_diff>
--- a/maps/legenda de assets.xlsx
+++ b/maps/legenda de assets.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">Parede1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parede1_2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">void</t>
   </si>
   <si>
     <t xml:space="preserve">parede_vermelha_grade_1</t>
@@ -40,10 +37,10 @@
     <t xml:space="preserve">parede_vermelha_esqueleto1_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Parede2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parede2_2</t>
+    <t xml:space="preserve">parede?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pilar_baixo_largo</t>
   </si>
   <si>
     <t xml:space="preserve">Portao_pedra1</t>
@@ -58,7 +55,13 @@
     <t xml:space="preserve">Portao_pedra3</t>
   </si>
   <si>
-    <t xml:space="preserve">Parede3_1</t>
+    <t xml:space="preserve">paralelepipedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao2</t>
   </si>
   <si>
     <t xml:space="preserve">bueiro_c_agua</t>
@@ -67,16 +70,25 @@
     <t xml:space="preserve">bueiro_s_agua</t>
   </si>
   <si>
-    <t xml:space="preserve">Parede4_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parede4_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parede_tijolo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chao_cinza</t>
+    <t xml:space="preserve">piso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao7</t>
   </si>
   <si>
     <t xml:space="preserve">Parede_verde</t>
@@ -89,11 +101,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,13 +124,22 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,62 +148,44 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF50200C"/>
+        <bgColor rgb="FF443205"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3838"/>
+        <bgColor rgb="FFED4C05"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF443205"/>
-        <bgColor rgb="FF472702"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF50200C"/>
-        <bgColor rgb="FF4B2204"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3838"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF472702"/>
-        <bgColor rgb="FF492300"/>
+        <bgColor rgb="FF50200C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF706E0C"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF492300"/>
-        <bgColor rgb="FF4B2204"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF5B277D"/>
+        <bgColor rgb="FF6B5E9B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6B5E9B"/>
+        <bgColor rgb="FF3465A4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5983B0"/>
+        <bgColor rgb="FF6B5E9B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF224B12"/>
         <bgColor rgb="FF383D3C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1E6A39"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4B2204"/>
-        <bgColor rgb="FF492300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3B160E"/>
-        <bgColor rgb="FF4B2204"/>
       </patternFill>
     </fill>
     <fill>
@@ -192,8 +196,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF3465A4"/>
+        <bgColor rgb="FF6B5E9B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B277D"/>
+        <bgColor rgb="FF660066"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF168253"/>
+        <bgColor rgb="FF127622"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED4C05"/>
+        <bgColor rgb="FFFF3838"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF127622"/>
+        <bgColor rgb="FF168253"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FF008080"/>
+        <bgColor rgb="FF168253"/>
       </patternFill>
     </fill>
   </fills>
@@ -231,16 +265,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,19 +286,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -268,23 +302,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,25 +343,25 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3838"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF50200C"/>
-      <rgbColor rgb="FF1E6A39"/>
+      <rgbColor rgb="FF127622"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF706E0C"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF168253"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF5983B0"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF472702"/>
+      <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
@@ -328,7 +370,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF4B2204"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
@@ -339,19 +381,19 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF3838"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FFED4C05"/>
+      <rgbColor rgb="FF6B5E9B"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF00A933"/>
-      <rgbColor rgb="FF3B160E"/>
+      <rgbColor rgb="FF224B12"/>
       <rgbColor rgb="FF443205"/>
-      <rgbColor rgb="FF492300"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF5B277D"/>
       <rgbColor rgb="FF383D3C"/>
@@ -365,98 +407,122 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D4:K14"/>
+  <dimension ref="C4:K14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="28.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="56.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="24.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="29.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.2"/>
   </cols>
   <sheetData>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="4" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="6" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="6" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="G9" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="13" t="s">
+    <row r="12" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>19</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mapa multiandar e mais algumas alterações
</commit_message>
<xml_diff>
--- a/maps/legenda de assets.xlsx
+++ b/maps/legenda de assets.xlsx
@@ -20,21 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t xml:space="preserve">void</t>
   </si>
   <si>
-    <t xml:space="preserve">parede_vermelha_grade_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parede_vermelha_grade_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parede_vermelha_esqueleto1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parede_vermelha_esqueleto1_2</t>
+    <t xml:space="preserve">parede11_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parede11_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parede11_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parede11_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parede11_5</t>
   </si>
   <si>
     <t xml:space="preserve">parede?</t>
@@ -43,16 +46,28 @@
     <t xml:space="preserve">pilar_baixo_largo</t>
   </si>
   <si>
-    <t xml:space="preserve">Portao_pedra1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portao_pedra2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portao_pedra4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portao_pedra3</t>
+    <t xml:space="preserve">escada_dupla_subir_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_subir_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_descer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_descer_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_subir_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_subir_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_descer_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_descer_4</t>
   </si>
   <si>
     <t xml:space="preserve">paralelepipedo</t>
@@ -61,19 +76,31 @@
     <t xml:space="preserve">chao1</t>
   </si>
   <si>
+    <t xml:space="preserve">escada_dupla_subir_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_subir_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_descer_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escada_dupla_descer_6</t>
+  </si>
+  <si>
     <t xml:space="preserve">chao2</t>
   </si>
   <si>
+    <t xml:space="preserve">piso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chao3</t>
+  </si>
+  <si>
     <t xml:space="preserve">bueiro_c_agua</t>
   </si>
   <si>
     <t xml:space="preserve">bueiro_s_agua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">piso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chao3</t>
   </si>
   <si>
     <t xml:space="preserve">chao4</t>
@@ -137,6 +164,7 @@
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -154,12 +182,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3838"/>
-        <bgColor rgb="FFED4C05"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF443205"/>
         <bgColor rgb="FF50200C"/>
       </patternFill>
@@ -172,6 +194,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF4000"/>
+        <bgColor rgb="FFED4C05"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF6B5E9B"/>
         <bgColor rgb="FF3465A4"/>
       </patternFill>
@@ -184,6 +212,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF3465A4"/>
+        <bgColor rgb="FF6B5E9B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF224B12"/>
         <bgColor rgb="FF383D3C"/>
       </patternFill>
@@ -196,12 +230,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3465A4"/>
-        <bgColor rgb="FF6B5E9B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF5B277D"/>
         <bgColor rgb="FF660066"/>
       </patternFill>
@@ -215,7 +243,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFED4C05"/>
-        <bgColor rgb="FFFF3838"/>
+        <bgColor rgb="FFFF4000"/>
       </patternFill>
     </fill>
     <fill>
@@ -298,7 +326,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,7 +334,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,7 +371,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF3838"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -407,15 +435,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C4:K14"/>
+  <dimension ref="C4:L14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="K6:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="56.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.19921875" defaultRowHeight="56.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.19"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -428,101 +456,131 @@
       <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>10</v>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>15</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
acrescentado alguns assets e otimização monstruosa no carregamento dos mapas, acrescentado classe para o player
</commit_message>
<xml_diff>
--- a/maps/legenda de assets.xlsx
+++ b/maps/legenda de assets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t xml:space="preserve">void</t>
   </si>
@@ -103,22 +103,130 @@
     <t xml:space="preserve">bueiro_s_agua</t>
   </si>
   <si>
+    <t xml:space="preserve">parede_horizontal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parede_direita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parede_esquerda</t>
+  </si>
+  <si>
     <t xml:space="preserve">chao4</t>
   </si>
   <si>
     <t xml:space="preserve">chao5</t>
   </si>
   <si>
-    <t xml:space="preserve">escada</t>
+    <t xml:space="preserve">estrutura_central_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_7</t>
   </si>
   <si>
     <t xml:space="preserve">chao6</t>
   </si>
   <si>
+    <t xml:space="preserve">estrutura_central_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_14</t>
+  </si>
+  <si>
     <t xml:space="preserve">chao7</t>
   </si>
   <si>
-    <t xml:space="preserve">Parede_verde</t>
+    <t xml:space="preserve">estrutura_central_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estrutura_central_35</t>
   </si>
 </sst>
 </file>
@@ -167,7 +275,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,7 +303,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
-        <bgColor rgb="FFED4C05"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -230,6 +338,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFE8A202"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFBF0041"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF0041"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF5B277D"/>
         <bgColor rgb="FF660066"/>
       </patternFill>
@@ -242,19 +368,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFED4C05"/>
-        <bgColor rgb="FFFF4000"/>
+        <fgColor rgb="FFE8A202"/>
+        <bgColor rgb="FFFF8000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF127622"/>
-        <bgColor rgb="FF168253"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00A933"/>
         <bgColor rgb="FF168253"/>
       </patternFill>
     </fill>
@@ -293,7 +413,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -338,11 +458,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,7 +474,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,7 +499,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF4000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -381,7 +509,7 @@
       <rgbColor rgb="FF127622"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF706E0C"/>
-      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FFBF0041"/>
       <rgbColor rgb="FF168253"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF5983B0"/>
@@ -413,15 +541,15 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFED4C05"/>
+      <rgbColor rgb="FFE8A202"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FF6B5E9B"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF224B12"/>
       <rgbColor rgb="FF443205"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF5B277D"/>
       <rgbColor rgb="FF383D3C"/>
@@ -435,10 +563,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C4:L14"/>
+  <dimension ref="C4:AO16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="K6:L8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.19921875" defaultRowHeight="56.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,43 +672,225 @@
       <c r="I10" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="K10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>27</v>
+      <c r="D11" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="D12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="0"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
+      <c r="V12" s="0"/>
+      <c r="W12" s="0"/>
+      <c r="X12" s="0"/>
+      <c r="Y12" s="0"/>
+      <c r="Z12" s="0"/>
+      <c r="AA12" s="0"/>
+      <c r="AB12" s="0"/>
+      <c r="AC12" s="0"/>
+      <c r="AD12" s="0"/>
+      <c r="AE12" s="0"/>
+      <c r="AF12" s="0"/>
+      <c r="AG12" s="0"/>
+      <c r="AH12" s="0"/>
+      <c r="AI12" s="0"/>
+      <c r="AJ12" s="0"/>
+      <c r="AK12" s="0"/>
+      <c r="AL12" s="0"/>
+      <c r="AM12" s="0"/>
+      <c r="AN12" s="0"/>
+      <c r="AO12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="D13" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="Z13" s="0"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="0"/>
+      <c r="AC13" s="0"/>
+      <c r="AD13" s="0"/>
+      <c r="AE13" s="0"/>
+      <c r="AF13" s="0"/>
+      <c r="AG13" s="0"/>
+      <c r="AH13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>32</v>
+      <c r="D14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="0"/>
+      <c r="O14" s="0"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
+      <c r="V14" s="0"/>
+      <c r="W14" s="0"/>
+      <c r="X14" s="0"/>
+      <c r="Y14" s="0"/>
+      <c r="Z14" s="0"/>
+      <c r="AA14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" s="0"/>
+      <c r="O15" s="0"/>
+      <c r="P15" s="0"/>
+      <c r="Q15" s="0"/>
+      <c r="R15" s="0"/>
+      <c r="S15" s="0"/>
+      <c r="T15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementado sistema de portas e passagens secretas
</commit_message>
<xml_diff>
--- a/maps/legenda de assets.xlsx
+++ b/maps/legenda de assets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t xml:space="preserve">void</t>
   </si>
@@ -139,6 +139,9 @@
     <t xml:space="preserve">estrutura_central_7</t>
   </si>
   <si>
+    <t xml:space="preserve">porta_grade_ch5</t>
+  </si>
+  <si>
     <t xml:space="preserve">chao6</t>
   </si>
   <si>
@@ -187,6 +190,9 @@
     <t xml:space="preserve">estrutura_central_21</t>
   </si>
   <si>
+    <t xml:space="preserve">porta_madeira_ch4</t>
+  </si>
+  <si>
     <t xml:space="preserve">estrutura_central_22</t>
   </si>
   <si>
@@ -227,6 +233,12 @@
   </si>
   <si>
     <t xml:space="preserve">estrutura_central_35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tocha_par_hor_torta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tocha_par_hor</t>
   </si>
 </sst>
 </file>
@@ -236,7 +248,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -274,8 +286,15 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,7 +322,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF3838"/>
       </patternFill>
     </fill>
     <fill>
@@ -333,7 +352,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF383D3C"/>
-        <bgColor rgb="FF443205"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
     <fill>
@@ -374,8 +393,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF333333"/>
+        <bgColor rgb="FF383D3C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF127622"/>
         <bgColor rgb="FF168253"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFA6"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3838"/>
+        <bgColor rgb="FFFF4000"/>
       </patternFill>
     </fill>
   </fills>
@@ -413,7 +456,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,7 +525,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,7 +573,7 @@
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF5983B0"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFF3838"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -532,27 +591,27 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFE8A202"/>
       <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FF6B5E9B"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF383D3C"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF224B12"/>
       <rgbColor rgb="FF443205"/>
       <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF5B277D"/>
-      <rgbColor rgb="FF383D3C"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -563,18 +622,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C4:AO16"/>
+  <dimension ref="C4:AO18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12:G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.19921875" defaultRowHeight="56.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.328125" defaultRowHeight="85.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="15.31"/>
   </cols>
   <sheetData>
-    <row r="4" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
@@ -614,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
@@ -628,7 +687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
@@ -648,7 +707,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
@@ -659,7 +718,7 @@
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
@@ -682,7 +741,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
@@ -690,7 +749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
@@ -719,7 +778,9 @@
         <v>38</v>
       </c>
       <c r="N12" s="0"/>
-      <c r="O12" s="0"/>
+      <c r="O12" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="P12" s="0"/>
       <c r="Q12" s="0"/>
       <c r="R12" s="0"/>
@@ -747,33 +808,33 @@
       <c r="AN12" s="0"/>
       <c r="AO12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>39</v>
+      <c r="D13" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N13" s="0"/>
       <c r="O13" s="0"/>
@@ -797,36 +858,38 @@
       <c r="AG13" s="0"/>
       <c r="AH13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N14" s="0"/>
-      <c r="O14" s="0"/>
+      <c r="O14" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="P14" s="0"/>
       <c r="Q14" s="0"/>
       <c r="R14" s="0"/>
@@ -840,27 +903,27 @@
       <c r="Z14" s="0"/>
       <c r="AA14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G15" s="16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="N15" s="0"/>
       <c r="O15" s="0"/>
@@ -870,27 +933,35 @@
       <c r="S15" s="0"/>
       <c r="T15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G16" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O18" s="21" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP implementação do segundo puzzle e teleport para o jardim
</commit_message>
<xml_diff>
--- a/maps/legenda de assets.xlsx
+++ b/maps/legenda de assets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t xml:space="preserve">void</t>
   </si>
@@ -214,6 +214,12 @@
     <t xml:space="preserve">estrutura_central_28</t>
   </si>
   <si>
+    <t xml:space="preserve">teleport_machine_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teleport_machine_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">estrutura_central_29</t>
   </si>
   <si>
@@ -236,6 +242,18 @@
   </si>
   <si>
     <t xml:space="preserve">tocha_par_hor_torta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teleport_machine_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teleport_machine_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teleport_machine_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teleport_machine_6</t>
   </si>
   <si>
     <t xml:space="preserve">tocha_par_hor</t>
@@ -294,7 +312,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +425,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFA6"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -456,7 +480,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,6 +566,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -624,8 +652,8 @@
   </sheetPr>
   <dimension ref="C4:AO18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.328125" defaultRowHeight="85.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -934,34 +962,54 @@
       <c r="T15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C16" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G16" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="O16" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="O18" s="21" t="s">
-        <v>72</v>
+      <c r="C18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O18" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>